<commit_message>
Added 2 Models from VSR for Engines
The OMS-L and Sepatron
</commit_message>
<xml_diff>
--- a/Notes/Engines.xlsx
+++ b/Notes/Engines.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="284">
   <si>
     <t>Name</t>
   </si>
@@ -891,12 +891,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -911,8 +917,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,9 +939,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H104" totalsRowShown="0">
-  <autoFilter ref="A1:H104"/>
-  <sortState ref="A70:H84">
-    <sortCondition ref="A1:A84"/>
+  <autoFilter ref="A1:H104">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Squad"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A17:H88">
+    <sortCondition ref="G1:G104"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
@@ -1215,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1239,7 @@
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1257,7 +1270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -1274,7 +1287,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -1291,7 +1304,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1308,7 +1321,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -1325,7 +1338,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -1342,7 +1355,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -1379,7 +1392,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -1396,7 +1409,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>212</v>
       </c>
@@ -1410,7 +1423,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -1424,7 +1437,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -1438,7 +1451,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>218</v>
       </c>
@@ -1452,7 +1465,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>220</v>
       </c>
@@ -1466,7 +1479,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>222</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>224</v>
       </c>
@@ -1493,191 +1506,194 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" t="s">
-        <v>183</v>
-      </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="H18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>103</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>132</v>
+        <v>101</v>
+      </c>
+      <c r="H20" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
-        <v>178</v>
-      </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>119</v>
+      </c>
+      <c r="H22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>121</v>
+      </c>
+      <c r="H23" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C24" t="s">
         <v>68</v>
       </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>88</v>
-      </c>
-      <c r="H26" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="G27" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>68</v>
@@ -1685,622 +1701,625 @@
       <c r="D28" t="s">
         <v>94</v>
       </c>
+      <c r="E28" t="s">
+        <v>179</v>
+      </c>
       <c r="G28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H28" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="D29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" t="s">
-        <v>182</v>
-      </c>
       <c r="G29" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="H29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>242</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>242</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
       <c r="G31" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H31" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
       <c r="G32" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="H32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="E33" t="s">
-        <v>181</v>
-      </c>
       <c r="G33" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="C34" t="s">
         <v>68</v>
       </c>
+      <c r="D34" t="s">
+        <v>94</v>
+      </c>
       <c r="G34" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="H34" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
         <v>68</v>
       </c>
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
         <v>68</v>
       </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" t="s">
+        <v>182</v>
+      </c>
       <c r="G36" t="s">
-        <v>99</v>
-      </c>
-      <c r="H36" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>68</v>
       </c>
       <c r="G37" t="s">
-        <v>101</v>
-      </c>
-      <c r="H37" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
         <v>68</v>
       </c>
+      <c r="E38" t="s">
+        <v>178</v>
+      </c>
       <c r="G38" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
       </c>
       <c r="C39" t="s">
         <v>68</v>
       </c>
+      <c r="E39" t="s">
+        <v>184</v>
+      </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="H40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
       </c>
       <c r="G41" t="s">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="H41" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
         <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>106</v>
+        <v>133</v>
+      </c>
+      <c r="H42" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>68</v>
       </c>
       <c r="G43" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
         <v>68</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G44" t="s">
-        <v>107</v>
-      </c>
-      <c r="H44" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
         <v>68</v>
       </c>
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
       <c r="G45" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
         <v>68</v>
       </c>
       <c r="G46" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="C47" t="s">
         <v>68</v>
       </c>
+      <c r="D47" t="s">
+        <v>94</v>
+      </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="G47" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
         <v>68</v>
       </c>
-      <c r="E48" t="s">
-        <v>186</v>
+      <c r="D48" t="s">
+        <v>94</v>
       </c>
       <c r="G48" t="s">
-        <v>136</v>
+        <v>90</v>
+      </c>
+      <c r="H48" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
         <v>68</v>
       </c>
-      <c r="E49" t="s">
-        <v>185</v>
-      </c>
       <c r="G49" t="s">
-        <v>185</v>
+        <v>85</v>
+      </c>
+      <c r="H49" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
         <v>68</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G50" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
         <v>68</v>
       </c>
-      <c r="D51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" t="s">
-        <v>179</v>
-      </c>
       <c r="G51" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
         <v>68</v>
       </c>
-      <c r="D52" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" t="s">
-        <v>179</v>
-      </c>
       <c r="G52" t="s">
-        <v>121</v>
-      </c>
-      <c r="H52" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
         <v>68</v>
       </c>
-      <c r="D53" t="s">
-        <v>94</v>
+      <c r="E53" t="s">
+        <v>183</v>
       </c>
       <c r="G53" t="s">
-        <v>123</v>
-      </c>
-      <c r="H53" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="D54" t="s">
-        <v>94</v>
+      <c r="E54" t="s">
+        <v>181</v>
       </c>
       <c r="G54" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
         <v>68</v>
       </c>
-      <c r="D55" t="s">
-        <v>94</v>
-      </c>
       <c r="G55" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s">
         <v>68</v>
       </c>
-      <c r="E56" t="s">
-        <v>180</v>
-      </c>
       <c r="G56" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C57" t="s">
         <v>68</v>
       </c>
       <c r="G57" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H57" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
         <v>68</v>
       </c>
+      <c r="E58" t="s">
+        <v>130</v>
+      </c>
       <c r="G58" t="s">
-        <v>119</v>
-      </c>
-      <c r="H58" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
         <v>68</v>
       </c>
+      <c r="E59" t="s">
+        <v>185</v>
+      </c>
       <c r="G59" t="s">
-        <v>55</v>
-      </c>
-      <c r="H59" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
         <v>68</v>
       </c>
-      <c r="E60" t="s">
-        <v>130</v>
+      <c r="D60" t="s">
+        <v>94</v>
       </c>
       <c r="G60" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="H60" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
         <v>68</v>
       </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
       <c r="G61" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="B62" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>116</v>
+        <v>97</v>
+      </c>
+      <c r="H62" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>242</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
-      <c r="F63" t="s">
-        <v>6</v>
+      <c r="G63" t="s">
+        <v>243</v>
+      </c>
+      <c r="H63" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
         <v>68</v>
       </c>
       <c r="F64" t="s">
-        <v>140</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
         <v>68</v>
       </c>
       <c r="F65" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -2314,7 +2333,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2328,7 +2347,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>144</v>
       </c>
@@ -2342,7 +2361,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>148</v>
       </c>
@@ -2356,7 +2375,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -2370,7 +2389,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2384,7 +2403,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2398,7 +2417,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>188</v>
       </c>
@@ -2412,7 +2431,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2426,7 +2445,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2437,7 +2456,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -2451,7 +2470,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -2465,7 +2484,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -2479,7 +2498,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>191</v>
       </c>
@@ -2493,7 +2512,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2504,7 +2523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>190</v>
       </c>
@@ -2518,7 +2537,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>192</v>
       </c>
@@ -2529,7 +2548,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -2543,7 +2562,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>233</v>
       </c>
@@ -2557,7 +2576,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>189</v>
       </c>
@@ -2568,7 +2587,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>233</v>
       </c>
@@ -2585,7 +2604,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>188</v>
       </c>
@@ -2604,22 +2623,19 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="B88" t="s">
-        <v>242</v>
+        <v>142</v>
       </c>
       <c r="C88" t="s">
         <v>68</v>
       </c>
-      <c r="G88" t="s">
-        <v>243</v>
-      </c>
-      <c r="H88" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>255</v>
       </c>
@@ -2630,7 +2646,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>258</v>
       </c>
@@ -2641,7 +2657,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>259</v>
       </c>
@@ -2652,7 +2668,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>261</v>
       </c>
@@ -2663,7 +2679,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>261</v>
       </c>
@@ -2677,7 +2693,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>264</v>
       </c>
@@ -2688,7 +2704,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>266</v>
       </c>
@@ -2699,7 +2715,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>268</v>
       </c>
@@ -2710,7 +2726,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>270</v>
       </c>
@@ -2721,7 +2737,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>272</v>
       </c>
@@ -2732,7 +2748,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>272</v>
       </c>
@@ -2746,7 +2762,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>276</v>
       </c>
@@ -2757,7 +2773,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>266</v>
       </c>
@@ -2771,7 +2787,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>266</v>
       </c>
@@ -2785,7 +2801,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>280</v>
       </c>
@@ -2796,7 +2812,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>282</v>
       </c>

</xml_diff>